<commit_message>
Cập nhật tạo examSlot
</commit_message>
<xml_diff>
--- a/demoImportExcelFile/Book1.xlsx
+++ b/demoImportExcelFile/Book1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>StudentID</t>
   </si>
@@ -28,31 +28,19 @@
     <t>SE171018</t>
   </si>
   <si>
-    <t xml:space="preserve">R0010          </t>
+    <t xml:space="preserve">R0025     </t>
   </si>
   <si>
     <t>SE170525</t>
   </si>
   <si>
-    <t xml:space="preserve">R0011          </t>
-  </si>
-  <si>
     <t>SE171010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R0012          </t>
   </si>
   <si>
     <t>SE170545</t>
   </si>
   <si>
-    <t xml:space="preserve">R0013          </t>
-  </si>
-  <si>
     <t>SE170540</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R0014          </t>
   </si>
 </sst>
 </file>
@@ -1001,7 +989,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="2"/>
@@ -1038,7 +1026,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1046,10 +1034,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1057,10 +1045,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1068,10 +1056,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>1</v>

</xml_diff>